<commit_message>
Added support for vector database
</commit_message>
<xml_diff>
--- a/src/data/train_dataset.xlsx
+++ b/src/data/train_dataset.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20401"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC9493A-0609-4573-A93C-C0045978DE46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -13,17 +14,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$E$2734</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -11628,7 +11618,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11824,6 +11814,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -11859,6 +11866,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -12034,7 +12058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2734"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A412" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -15393,7 +15417,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A419" s="4" t="s">
         <v>3429</v>
       </c>
@@ -33914,7 +33938,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2734"/>
+  <autoFilter ref="A1:E2734" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>